<commit_message>
code seems right -- can't do slope beyond cthresh
</commit_message>
<xml_diff>
--- a/working/CrizerPFAS/dataguide-DC-hep.xlsx
+++ b/working/CrizerPFAS/dataguide-DC-hep.xlsx
@@ -8,17 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\invitrotkstats\working\CrizerPFAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F1348A-FE03-4BFD-8F4F-E01C0CD36DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC8CAB0-A807-426E-BCDA-09D54FBDA4FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{FBD20694-86E7-4EA8-9E3F-9E73DC7D54DE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FBD20694-86E7-4EA8-9E3F-9E73DC7D54DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Use" sheetId="1" r:id="rId1"/>
     <sheet name="Ignore" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="187">
   <si>
     <t>File</t>
   </si>
@@ -574,18 +571,12 @@
     <t>3-Perfluoroheptylpropanoic acid (7:3 FTCA)</t>
   </si>
   <si>
-    <t>N-Ethylperfluorooctanesulfonamide (NEtFOSA)</t>
-  </si>
-  <si>
     <t>9-H-Perfluorononanoic acid (9H-PFNA)</t>
   </si>
   <si>
     <t>Perfluoro(2-ethoxyethane)sulfonic acid</t>
   </si>
   <si>
-    <t>Potassium perfluorooctanoate (KPFOA)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> M9PFNA</t>
   </si>
   <si>
@@ -599,6 +590,12 @@
   </si>
   <si>
     <t>Sample Text</t>
+  </si>
+  <si>
+    <t>Num.Rows</t>
+  </si>
+  <si>
+    <t>Potassium perfluorooctanoate</t>
   </si>
 </sst>
 </file>
@@ -811,7 +808,7 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{AB4D46B3-DFA6-4315-AA8A-25CEF954E896}"/>
     <cellStyle name="Normal 2 2" xfId="2" xr:uid="{25EB36AE-F99D-4E2F-8ACF-1C6A1F319CD6}"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="16">
     <dxf>
       <font>
         <b val="0"/>
@@ -824,12 +821,22 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="9"/>
-        <color auto="1"/>
+        <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1058,6 +1065,25 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -1073,32 +1099,14 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Summary"/>
-      <sheetName val="Clint Summary Sheet"/>
-      <sheetName val="Ref Compounds RAW"/>
-      <sheetName val="PFAS RAW"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A9B8EE4D-D583-4D2F-BFFA-E810C09BBB35}" name="Table1" displayName="Table1" ref="A1:M46" totalsRowShown="0" headerRowDxfId="14" dataDxfId="0">
-  <autoFilter ref="A1:M46" xr:uid="{A9B8EE4D-D583-4D2F-BFFA-E810C09BBB35}"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A9B8EE4D-D583-4D2F-BFFA-E810C09BBB35}" name="Table1" displayName="Table1" ref="A1:N46" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A1:N46" xr:uid="{A9B8EE4D-D583-4D2F-BFFA-E810C09BBB35}"/>
+  <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{F31FEEE7-5670-480B-8D69-C837166A4265}" name="File" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{E35EDAE4-7B2F-445D-ADCF-4312C026D29C}" name="Sheet" dataDxfId="12"/>
     <tableColumn id="3" xr3:uid="{7CC1D113-233F-4125-9B3C-BF06263823E3}" name="Skip.Rows" dataDxfId="11"/>
+    <tableColumn id="14" xr3:uid="{6956AC45-AB3B-480B-BC09-88D4DBE96CF4}" name="Num.Rows" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{0D00559A-0EA4-4B43-936B-FF54C5967A3B}" name="Date" dataDxfId="10"/>
     <tableColumn id="5" xr3:uid="{30C20B5C-3D26-454B-9FAF-9ADF4ABEFC49}" name="Chemical.ID" dataDxfId="9"/>
     <tableColumn id="6" xr3:uid="{99D37553-9172-43E7-B22F-BCBAB5D595A4}" name="ISTD.Name" dataDxfId="8"/>
@@ -1411,10 +1419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4EAA0A0-5807-4BE5-8864-D0C317F02936}">
-  <dimension ref="A1:M54"/>
+  <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="L47" sqref="L47"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1422,18 +1430,19 @@
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="30.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.81640625" customWidth="1"/>
-    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" customWidth="1"/>
+    <col min="5" max="5" width="7.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="55.81640625" customWidth="1"/>
+    <col min="7" max="7" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1443,38 +1452,41 @@
       <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="J1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -1484,38 +1496,39 @@
       <c r="C2" s="4">
         <v>4</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>18</v>
+      <c r="G2" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>25</v>
       </c>
@@ -1525,38 +1538,39 @@
       <c r="C3" s="4">
         <v>4</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>18</v>
+      <c r="G3" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>26</v>
       </c>
@@ -1566,38 +1580,39 @@
       <c r="C4" s="4">
         <v>4</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>18</v>
+      <c r="G4" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -1607,38 +1622,39 @@
       <c r="C5" s="4">
         <v>4</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="F5" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>18</v>
+      <c r="G5" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>55</v>
       </c>
@@ -1648,38 +1664,39 @@
       <c r="C6" s="4">
         <v>4</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4"/>
+      <c r="E6" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="F6" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>18</v>
+      <c r="G6" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>54</v>
       </c>
@@ -1689,38 +1706,39 @@
       <c r="C7" s="4">
         <v>4</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="F7" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>18</v>
+      <c r="G7" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>53</v>
       </c>
@@ -1730,38 +1748,39 @@
       <c r="C8" s="4">
         <v>4</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4"/>
+      <c r="E8" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="F8" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>18</v>
+      <c r="G8" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>52</v>
       </c>
@@ -1771,38 +1790,39 @@
       <c r="C9" s="4">
         <v>4</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4"/>
+      <c r="E9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>18</v>
+      <c r="G9" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>51</v>
       </c>
@@ -1812,38 +1832,39 @@
       <c r="C10" s="4">
         <v>4</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4"/>
+      <c r="E10" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>18</v>
+      <c r="G10" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>50</v>
       </c>
@@ -1853,38 +1874,39 @@
       <c r="C11" s="4">
         <v>4</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4"/>
+      <c r="E11" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="F11" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>18</v>
+      <c r="G11" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>49</v>
       </c>
@@ -1894,38 +1916,39 @@
       <c r="C12" s="4">
         <v>4</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4"/>
+      <c r="E12" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="F12" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>18</v>
+      <c r="G12" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L12" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L12" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>48</v>
       </c>
@@ -1935,38 +1958,39 @@
       <c r="C13" s="4">
         <v>4</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4"/>
+      <c r="E13" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="F13" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>18</v>
+      <c r="G13" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L13" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M13" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>47</v>
       </c>
@@ -1976,38 +2000,39 @@
       <c r="C14" s="4">
         <v>4</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4"/>
+      <c r="E14" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="F14" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>18</v>
+      <c r="G14" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L14" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>81</v>
       </c>
@@ -2017,38 +2042,39 @@
       <c r="C15" s="4">
         <v>4</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4"/>
+      <c r="E15" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="F15" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>18</v>
+      <c r="G15" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K15" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L15" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L15" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M15" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>46</v>
       </c>
@@ -2058,38 +2084,39 @@
       <c r="C16" s="4">
         <v>4</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4"/>
+      <c r="E16" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="F16" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>18</v>
+      <c r="G16" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M16" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>87</v>
       </c>
@@ -2099,38 +2126,39 @@
       <c r="C17" s="4">
         <v>4</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4"/>
+      <c r="E17" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="F17" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>18</v>
+      <c r="G17" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K17" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L17" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L17" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M17" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>45</v>
       </c>
@@ -2140,38 +2168,39 @@
       <c r="C18" s="4">
         <v>4</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4"/>
+      <c r="E18" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="F18" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>18</v>
+      <c r="G18" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L18" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L18" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M18" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>44</v>
       </c>
@@ -2181,38 +2210,39 @@
       <c r="C19" s="4">
         <v>4</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4"/>
+      <c r="E19" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="F19" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>18</v>
+      <c r="G19" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K19" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L19" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L19" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M19" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>43</v>
       </c>
@@ -2222,38 +2252,39 @@
       <c r="C20" s="4">
         <v>4</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="4"/>
+      <c r="E20" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="F20" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>18</v>
+      <c r="G20" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K20" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L20" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L20" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M20" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M20" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>42</v>
       </c>
@@ -2263,38 +2294,39 @@
       <c r="C21" s="4">
         <v>4</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="4"/>
+      <c r="E21" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="F21" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="F21" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>18</v>
+      <c r="G21" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K21" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L21" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M21" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>41</v>
       </c>
@@ -2304,38 +2336,39 @@
       <c r="C22" s="4">
         <v>4</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4"/>
+      <c r="E22" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="F22" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="F22" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>18</v>
+      <c r="G22" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K22" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L22" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L22" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M22" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>40</v>
       </c>
@@ -2345,38 +2378,39 @@
       <c r="C23" s="4">
         <v>4</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="4"/>
+      <c r="E23" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="F23" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="F23" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>18</v>
+      <c r="G23" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K23" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L23" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L23" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M23" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M23" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
         <v>39</v>
       </c>
@@ -2386,38 +2420,39 @@
       <c r="C24" s="12">
         <v>4</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="12"/>
+      <c r="E24" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="F24" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F24" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>18</v>
+      <c r="G24" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I24" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="J24" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K24" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K24" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L24" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="L24" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="M24" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M24" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N24" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
         <v>38</v>
       </c>
@@ -2427,38 +2462,39 @@
       <c r="C25" s="12">
         <v>4</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="12"/>
+      <c r="E25" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="F25" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="F25" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G25" s="14" t="s">
-        <v>18</v>
+      <c r="G25" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I25" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I25" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="J25" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K25" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K25" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L25" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="L25" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="M25" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M25" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N25" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
         <v>37</v>
       </c>
@@ -2468,38 +2504,39 @@
       <c r="C26" s="12">
         <v>4</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="12"/>
+      <c r="E26" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="F26" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="F26" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G26" s="14" t="s">
-        <v>18</v>
+      <c r="G26" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="H26" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I26" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I26" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="J26" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K26" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K26" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L26" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="L26" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="M26" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M26" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N26" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" s="11" t="s">
         <v>36</v>
       </c>
@@ -2509,38 +2546,39 @@
       <c r="C27" s="12">
         <v>4</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="12"/>
+      <c r="E27" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="F27" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F27" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>18</v>
+      <c r="G27" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="H27" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I27" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="J27" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K27" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K27" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L27" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="L27" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="M27" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M27" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N27" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" s="11" t="s">
         <v>35</v>
       </c>
@@ -2550,38 +2588,39 @@
       <c r="C28" s="12">
         <v>4</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="12"/>
+      <c r="E28" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="F28" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="F28" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G28" s="14" t="s">
-        <v>18</v>
+      <c r="G28" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I28" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I28" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="J28" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K28" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K28" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L28" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="L28" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="M28" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M28" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N28" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
         <v>34</v>
       </c>
@@ -2591,38 +2630,39 @@
       <c r="C29" s="12">
         <v>4</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="12"/>
+      <c r="E29" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="F29" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="F29" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" s="14" t="s">
-        <v>18</v>
+      <c r="G29" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="H29" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I29" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I29" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="J29" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K29" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K29" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L29" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="L29" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="M29" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M29" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N29" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" s="11" t="s">
         <v>33</v>
       </c>
@@ -2632,38 +2672,39 @@
       <c r="C30" s="12">
         <v>4</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="12"/>
+      <c r="E30" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="F30" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="F30" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G30" s="14" t="s">
-        <v>18</v>
+      <c r="G30" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="H30" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I30" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I30" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="J30" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K30" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K30" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L30" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="L30" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="M30" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M30" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N30" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" s="11" t="s">
         <v>32</v>
       </c>
@@ -2673,38 +2714,39 @@
       <c r="C31" s="12">
         <v>4</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="12"/>
+      <c r="E31" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="F31" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="F31" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G31" s="14" t="s">
-        <v>18</v>
+      <c r="G31" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="H31" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I31" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I31" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="J31" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K31" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K31" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L31" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="L31" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="M31" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M31" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N31" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" s="11" t="s">
         <v>31</v>
       </c>
@@ -2714,38 +2756,39 @@
       <c r="C32" s="12">
         <v>4</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="12"/>
+      <c r="E32" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="F32" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="F32" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G32" s="14" t="s">
-        <v>18</v>
+      <c r="G32" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="H32" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I32" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I32" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="J32" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K32" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K32" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L32" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="L32" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="M32" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M32" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N32" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" s="11" t="s">
         <v>30</v>
       </c>
@@ -2755,38 +2798,39 @@
       <c r="C33" s="12">
         <v>4</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="D33" s="12"/>
+      <c r="E33" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="F33" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="F33" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G33" s="14" t="s">
-        <v>18</v>
+      <c r="G33" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="H33" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I33" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I33" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="J33" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K33" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K33" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L33" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="L33" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="M33" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M33" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N33" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" s="11" t="s">
         <v>29</v>
       </c>
@@ -2796,38 +2840,39 @@
       <c r="C34" s="12">
         <v>4</v>
       </c>
-      <c r="D34" s="13" t="s">
+      <c r="D34" s="12"/>
+      <c r="E34" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="F34" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="F34" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G34" s="14" t="s">
-        <v>18</v>
+      <c r="G34" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="H34" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I34" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I34" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="J34" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K34" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K34" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L34" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="L34" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="M34" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M34" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N34" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" s="11" t="s">
         <v>124</v>
       </c>
@@ -2837,38 +2882,39 @@
       <c r="C35" s="12">
         <v>4</v>
       </c>
-      <c r="D35" s="13" t="s">
+      <c r="D35" s="12"/>
+      <c r="E35" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="F35" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="F35" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G35" s="14" t="s">
-        <v>18</v>
+      <c r="G35" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="H35" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I35" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I35" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="J35" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K35" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K35" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L35" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="L35" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="M35" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M35" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N35" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" s="11" t="s">
         <v>28</v>
       </c>
@@ -2878,38 +2924,39 @@
       <c r="C36" s="12">
         <v>4</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="D36" s="12"/>
+      <c r="E36" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="F36" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="F36" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G36" s="14" t="s">
-        <v>18</v>
+      <c r="G36" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="H36" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I36" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="I36" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="J36" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K36" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K36" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L36" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="L36" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="M36" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M36" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N36" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" s="11" t="s">
         <v>143</v>
       </c>
@@ -2919,38 +2966,39 @@
       <c r="C37" s="12">
         <v>4</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="D37" s="12"/>
+      <c r="E37" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="F37" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="F37" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G37" s="14" t="s">
-        <v>18</v>
+      <c r="G37" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="H37" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I37" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I37" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J37" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="J37" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K37" s="16" t="s">
+      <c r="K37" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L37" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="L37" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="M37" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M37" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N37" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" s="11" t="s">
         <v>144</v>
       </c>
@@ -2960,38 +3008,39 @@
       <c r="C38" s="12">
         <v>4</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="12"/>
+      <c r="E38" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="F38" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="F38" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G38" s="14" t="s">
-        <v>18</v>
+      <c r="G38" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="H38" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I38" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J38" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="J38" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K38" s="16" t="s">
+      <c r="K38" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L38" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="L38" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="M38" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M38" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N38" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39" s="11" t="s">
         <v>145</v>
       </c>
@@ -3001,38 +3050,39 @@
       <c r="C39" s="12">
         <v>4</v>
       </c>
-      <c r="D39" s="13" t="s">
+      <c r="D39" s="12"/>
+      <c r="E39" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="F39" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="F39" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G39" s="14" t="s">
-        <v>18</v>
+      <c r="G39" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="H39" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I39" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I39" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J39" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="J39" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K39" s="16" t="s">
+      <c r="K39" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L39" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="L39" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="M39" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M39" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N39" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40" s="11" t="s">
         <v>146</v>
       </c>
@@ -3042,38 +3092,39 @@
       <c r="C40" s="12">
         <v>4</v>
       </c>
-      <c r="D40" s="13" t="s">
+      <c r="D40" s="12"/>
+      <c r="E40" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="E40" s="7" t="s">
+      <c r="F40" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="F40" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G40" s="14" t="s">
-        <v>18</v>
+      <c r="G40" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="H40" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I40" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I40" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="J40" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K40" s="16" t="s">
+      <c r="K40" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L40" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="L40" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="M40" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M40" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N40" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A41" s="11" t="s">
         <v>147</v>
       </c>
@@ -3083,38 +3134,39 @@
       <c r="C41" s="12">
         <v>4</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="D41" s="12"/>
+      <c r="E41" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="E41" s="7" t="s">
+      <c r="F41" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="F41" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G41" s="14" t="s">
-        <v>18</v>
+      <c r="G41" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="H41" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I41" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I41" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="J41" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K41" s="16" t="s">
+      <c r="K41" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L41" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="L41" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="M41" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M41" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N41" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42" s="11" t="s">
         <v>148</v>
       </c>
@@ -3124,38 +3176,39 @@
       <c r="C42" s="12">
         <v>4</v>
       </c>
-      <c r="D42" s="13" t="s">
+      <c r="D42" s="12"/>
+      <c r="E42" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="F42" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="F42" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G42" s="14" t="s">
-        <v>18</v>
+      <c r="G42" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="H42" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I42" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I42" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J42" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="J42" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K42" s="16" t="s">
+      <c r="K42" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L42" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="L42" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="M42" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M42" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N42" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A43" s="11" t="s">
         <v>149</v>
       </c>
@@ -3165,38 +3218,39 @@
       <c r="C43" s="12">
         <v>4</v>
       </c>
-      <c r="D43" s="13" t="s">
+      <c r="D43" s="12"/>
+      <c r="E43" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="E43" s="7" t="s">
+      <c r="F43" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="F43" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G43" s="14" t="s">
-        <v>18</v>
+      <c r="G43" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="H43" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I43" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I43" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J43" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="J43" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K43" s="16" t="s">
+      <c r="K43" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L43" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="L43" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="M43" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M43" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N43" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A44" s="11" t="s">
         <v>150</v>
       </c>
@@ -3206,38 +3260,39 @@
       <c r="C44" s="12">
         <v>4</v>
       </c>
-      <c r="D44" s="13" t="s">
+      <c r="D44" s="12"/>
+      <c r="E44" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="F44" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="F44" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G44" s="14" t="s">
-        <v>18</v>
+      <c r="G44" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="H44" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I44" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I44" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J44" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="J44" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K44" s="16" t="s">
+      <c r="K44" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L44" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="L44" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="M44" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M44" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N44" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>153</v>
       </c>
@@ -3247,38 +3302,41 @@
       <c r="C45" s="4">
         <v>15</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="4">
+        <v>131</v>
+      </c>
+      <c r="E45" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="E45" s="18" t="s">
+      <c r="F45" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="F45" s="19" t="s">
+      <c r="G45" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="G45" s="4" t="s">
+      <c r="H45" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="H45" s="4" t="s">
+      <c r="I45" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="I45" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="J45" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K45" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="K45" s="4" t="s">
+      <c r="L45" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="L45" s="22" t="s">
+      <c r="M45" s="22" t="s">
         <v>171</v>
       </c>
-      <c r="M45" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N45" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>153</v>
       </c>
@@ -3286,40 +3344,43 @@
         <v>154</v>
       </c>
       <c r="C46" s="4">
-        <v>150</v>
-      </c>
-      <c r="D46" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="D46" s="4">
+        <v>131</v>
+      </c>
+      <c r="E46" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="E46" s="18" t="s">
+      <c r="F46" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="F46" s="19" t="s">
+      <c r="G46" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="G46" s="4" t="s">
+      <c r="H46" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="H46" s="4" t="s">
+      <c r="I46" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="I46" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J46" s="8" t="s">
+      <c r="J46" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K46" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="K46" s="4" t="s">
+      <c r="L46" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="L46" s="21" t="s">
-        <v>184</v>
-      </c>
-      <c r="M46" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M46" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="N46" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>153</v>
       </c>
@@ -3329,38 +3390,41 @@
       <c r="C47" s="4">
         <v>19</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" s="4">
+        <v>192</v>
+      </c>
+      <c r="E47" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="E47" s="18" t="s">
+      <c r="F47" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="F47" s="4" t="s">
+      <c r="G47" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="G47" s="4" t="s">
+      <c r="H47" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="H47" s="4" t="s">
+      <c r="I47" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="I47" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="J47" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K47" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="K47" s="4" t="s">
+      <c r="L47" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="L47" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="M47" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M47" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="N47" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
         <v>153</v>
       </c>
@@ -3370,38 +3434,41 @@
       <c r="C48" s="4">
         <v>607</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D48" s="4">
+        <v>192</v>
+      </c>
+      <c r="E48" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="E48" s="18" t="s">
+      <c r="F48" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="F48" s="4" t="s">
+      <c r="G48" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="G48" s="4" t="s">
+      <c r="H48" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="H48" s="4" t="s">
+      <c r="I48" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="I48" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="J48" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K48" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="K48" s="4" t="s">
+      <c r="L48" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="L48" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="M48" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M48" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="N48" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>153</v>
       </c>
@@ -3411,38 +3478,41 @@
       <c r="C49" s="4">
         <v>215</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D49" s="4">
+        <v>192</v>
+      </c>
+      <c r="E49" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="E49" s="18" t="s">
+      <c r="F49" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="F49" s="4" t="s">
+      <c r="G49" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="G49" s="4" t="s">
+      <c r="H49" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="H49" s="4" t="s">
+      <c r="I49" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="I49" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="J49" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K49" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="K49" s="4" t="s">
+      <c r="L49" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="L49" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="M49" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M49" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="N49" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>174</v>
       </c>
@@ -3452,38 +3522,41 @@
       <c r="C50" s="4">
         <v>826</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D50" s="4">
+        <v>160</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F50" t="s">
         <v>177</v>
       </c>
-      <c r="F50" t="s">
-        <v>182</v>
-      </c>
       <c r="G50" t="s">
+        <v>180</v>
+      </c>
+      <c r="H50" t="s">
         <v>173</v>
       </c>
-      <c r="H50" t="s">
+      <c r="I50" t="s">
         <v>170</v>
       </c>
-      <c r="I50" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="J50" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K50" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="K50" s="4" t="s">
+      <c r="L50" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="L50" t="s">
-        <v>186</v>
-      </c>
-      <c r="M50" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M50" t="s">
+        <v>184</v>
+      </c>
+      <c r="N50" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>174</v>
       </c>
@@ -3493,38 +3566,41 @@
       <c r="C51" s="4">
         <v>1154</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D51" s="4">
+        <v>160</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="E51" t="s">
-        <v>178</v>
-      </c>
       <c r="F51" t="s">
-        <v>183</v>
+        <v>64</v>
       </c>
       <c r="G51" t="s">
+        <v>181</v>
+      </c>
+      <c r="H51" t="s">
         <v>173</v>
       </c>
-      <c r="H51" t="s">
+      <c r="I51" t="s">
         <v>170</v>
       </c>
-      <c r="I51" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="J51" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K51" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="K51" s="4" t="s">
+      <c r="L51" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="L51" t="s">
-        <v>186</v>
-      </c>
-      <c r="M51" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M51" t="s">
+        <v>184</v>
+      </c>
+      <c r="N51" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>174</v>
       </c>
@@ -3534,38 +3610,41 @@
       <c r="C52" s="4">
         <v>334</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D52" s="4">
+        <v>160</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="E52" t="s">
-        <v>179</v>
-      </c>
       <c r="F52" t="s">
+        <v>178</v>
+      </c>
+      <c r="G52" t="s">
         <v>166</v>
       </c>
-      <c r="G52" t="s">
+      <c r="H52" t="s">
         <v>173</v>
       </c>
-      <c r="H52" t="s">
+      <c r="I52" t="s">
         <v>170</v>
       </c>
-      <c r="I52" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="J52" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K52" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="K52" s="4" t="s">
+      <c r="L52" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="L52" t="s">
-        <v>186</v>
-      </c>
-      <c r="M52" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M52" t="s">
+        <v>184</v>
+      </c>
+      <c r="N52" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>174</v>
       </c>
@@ -3575,38 +3654,41 @@
       <c r="C53" s="4">
         <v>6</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D53" s="4">
+        <v>160</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="E53" t="s">
-        <v>180</v>
-      </c>
       <c r="F53" t="s">
+        <v>179</v>
+      </c>
+      <c r="G53" t="s">
         <v>167</v>
       </c>
-      <c r="G53" t="s">
+      <c r="H53" t="s">
         <v>173</v>
       </c>
-      <c r="H53" t="s">
+      <c r="I53" t="s">
         <v>170</v>
       </c>
-      <c r="I53" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="J53" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K53" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="K53" s="4" t="s">
+      <c r="L53" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="L53" t="s">
-        <v>186</v>
-      </c>
-      <c r="M53" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M53" t="s">
+        <v>184</v>
+      </c>
+      <c r="N53" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>174</v>
       </c>
@@ -3616,34 +3698,37 @@
       <c r="C54" s="4">
         <v>498</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D54" s="4">
+        <v>160</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="E54" t="s">
-        <v>181</v>
-      </c>
       <c r="F54" t="s">
+        <v>186</v>
+      </c>
+      <c r="G54" t="s">
         <v>166</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H54" t="s">
         <v>173</v>
       </c>
-      <c r="H54" t="s">
+      <c r="I54" t="s">
         <v>170</v>
       </c>
-      <c r="I54" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="J54" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K54" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="K54" s="4" t="s">
+      <c r="L54" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="L54" t="s">
-        <v>186</v>
-      </c>
-      <c r="M54" s="20" t="s">
+      <c r="M54" t="s">
+        <v>184</v>
+      </c>
+      <c r="N54" s="20" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3701,7 +3786,7 @@
         <v>172</v>
       </c>
       <c r="L1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M1" s="20" t="s">
         <v>24</v>

</xml_diff>